<commit_message>
Updated wind 2025 FI
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="52">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -321,13 +321,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F84" activeCellId="0" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,7 +371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -395,7 +395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -418,7 +418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -466,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -507,7 +507,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -524,7 +524,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -542,7 +542,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -560,7 +560,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -577,7 +577,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -594,7 +594,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -611,7 +611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -629,7 +629,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -646,7 +646,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -663,7 +663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -681,7 +681,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -698,7 +698,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -715,7 +715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -733,7 +733,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -751,7 +751,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -769,7 +769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -788,7 +788,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -806,7 +806,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -823,7 +823,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -840,7 +840,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -874,7 +874,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -891,7 +891,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -908,7 +908,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -925,7 +925,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
@@ -942,7 +942,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
@@ -977,7 +977,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>28</v>
       </c>
@@ -994,7 +994,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>27</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>27</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>35</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>30</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>30</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>14</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>14</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>14</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>30</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>27</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>17</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>35</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>35</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>30</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>30</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>38</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>38</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>38</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>14</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>26</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
         <v>42</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>43</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>43</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>43</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>42</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>42</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>42</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>45</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>45</v>
       </c>
@@ -1938,9 +1938,21 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
+      <c r="A89" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>4500</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1"/>
@@ -2375,7 +2387,13 @@
       <c r="E162" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J88"/>
+  <autoFilter ref="A1:J88">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="FR00"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added SE03 industrial CHP.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$88</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$91</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="52">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -321,13 +321,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J162"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F84" activeCellId="0" sqref="F84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,7 +371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -395,7 +395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -418,7 +418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -466,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -507,7 +507,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -524,7 +524,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -542,7 +542,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -560,7 +560,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -577,7 +577,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -594,7 +594,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -611,7 +611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -629,7 +629,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -646,7 +646,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -663,7 +663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -681,7 +681,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -698,7 +698,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -715,7 +715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -733,7 +733,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -751,7 +751,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -769,7 +769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -788,7 +788,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -806,7 +806,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -823,7 +823,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -840,7 +840,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -874,7 +874,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -891,7 +891,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -908,7 +908,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -925,7 +925,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
@@ -942,7 +942,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
@@ -977,7 +977,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>28</v>
       </c>
@@ -994,7 +994,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -1143,14 +1143,13 @@
         <v>2025</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C44" s="3" t="s">
         <v>19</v>
       </c>
@@ -1160,16 +1159,14 @@
       <c r="E44" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="F44" s="1"/>
       <c r="H44" s="1" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="3"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>20</v>
       </c>
@@ -1180,16 +1177,16 @@
         <v>2025</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>33</v>
@@ -1202,12 +1199,13 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>35</v>
-      </c>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>33</v>
@@ -1215,15 +1213,15 @@
       <c r="E47" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="H47" s="1" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="F47" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
         <v>21</v>
       </c>
@@ -1235,12 +1233,12 @@
       </c>
       <c r="F48" s="1"/>
       <c r="H48" s="1" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>19</v>
@@ -1256,9 +1254,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>21</v>
@@ -1274,82 +1272,84 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="H51" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="H52" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F51" s="3" t="n">
+      <c r="D53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F53" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3" t="s">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3" t="n">
+      <c r="D54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F53" s="1" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F54" s="1" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>29</v>
@@ -1361,15 +1361,15 @@
         <v>2025</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>33</v>
@@ -1378,12 +1378,12 @@
         <v>2025</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="s">
-        <v>27</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>29</v>
@@ -1395,12 +1395,12 @@
         <v>2025</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="s">
-        <v>17</v>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>29</v>
@@ -1412,49 +1412,49 @@
         <v>2025</v>
       </c>
       <c r="F58" s="1" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F60" s="1" t="n">
         <v>1500</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="H59" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F60" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>12</v>
@@ -1462,17 +1462,16 @@
       <c r="E61" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F61" s="1"/>
       <c r="H61" s="1" t="n">
         <v>1500</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>12</v>
@@ -1480,16 +1479,16 @@
       <c r="E62" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="H62" s="1" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>12</v>
@@ -1497,16 +1496,17 @@
       <c r="E63" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F63" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F63" s="1"/>
+      <c r="H63" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>12</v>
@@ -1514,17 +1514,16 @@
       <c r="E64" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F64" s="1"/>
       <c r="H64" s="1" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>12</v>
@@ -1532,16 +1531,16 @@
       <c r="E65" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="H65" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F65" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>12</v>
@@ -1549,16 +1548,17 @@
       <c r="E66" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F66" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F66" s="1"/>
+      <c r="H66" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>12</v>
@@ -1566,70 +1566,69 @@
       <c r="E67" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F67" s="1"/>
       <c r="H67" s="1" t="n">
         <v>1500</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F68" s="1"/>
-      <c r="H68" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2040</v>
+      </c>
+      <c r="F68" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="F69" s="1"/>
       <c r="H69" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="H70" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E70" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F70" s="1" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>33</v>
@@ -1637,16 +1636,17 @@
       <c r="E71" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="F71" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F71" s="1"/>
+      <c r="H71" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>19</v>
+      <c r="C72" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>33</v>
@@ -1654,17 +1654,16 @@
       <c r="E72" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="H72" s="1" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F72" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>33</v>
@@ -1673,102 +1672,103 @@
         <v>2025</v>
       </c>
       <c r="F73" s="1" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>2040</v>
-      </c>
+        <v>2025</v>
+      </c>
+      <c r="F74" s="1"/>
       <c r="H74" s="1" t="n">
-        <v>12000</v>
+        <v>700</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="F75" s="1" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H76" s="1" t="n">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F76" s="1"/>
-      <c r="H76" s="1" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F77" s="1" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D78" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="3" t="n">
         <v>2040</v>
       </c>
+      <c r="F78" s="1"/>
       <c r="H78" s="1" t="n">
         <v>4000</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>43</v>
-      </c>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" s="3"/>
       <c r="C79" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>12</v>
@@ -1777,15 +1777,15 @@
         <v>2040</v>
       </c>
       <c r="F79" s="1" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>21</v>
+      <c r="C80" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>12</v>
@@ -1793,17 +1793,16 @@
       <c r="E80" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F80" s="1"/>
       <c r="H80" s="1" t="n">
         <v>4000</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>12</v>
@@ -1811,16 +1810,16 @@
       <c r="E81" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="H81" s="1" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F81" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>12</v>
@@ -1828,175 +1827,198 @@
       <c r="E82" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F82" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F82" s="1"/>
+      <c r="H82" s="1" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H83" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F84" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F83" s="1"/>
-      <c r="H83" s="1" t="n">
+      <c r="D85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="H85" s="1" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3" t="s">
+      <c r="B86" s="3"/>
+      <c r="C86" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E84" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F84" s="3" t="n">
+      <c r="D86" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F86" s="3" t="n">
         <v>52000</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3" t="s">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E85" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F85" s="3" t="n">
+      <c r="D87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F87" s="3" t="n">
         <v>48000</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E86" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F86" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F87" s="1" t="n">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="F88" s="1" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F89" s="1" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E90" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F90" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F89" s="0" t="n">
+      <c r="D91" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F91" s="1" t="n">
         <v>4500</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-    </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3"/>
+      <c r="A92" s="1"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="1"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1"/>
+      <c r="A94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1"/>
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="1"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
@@ -2062,6 +2084,7 @@
       <c r="A107" s="1"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
+      <c r="F107" s="1"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
@@ -2073,17 +2096,18 @@
       <c r="A109" s="1"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="1"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
+      <c r="F110" s="1"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
+      <c r="F111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1"/>
@@ -2094,23 +2118,23 @@
       <c r="A113" s="1"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
-      <c r="F114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
+      <c r="F115" s="1"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
+      <c r="F116" s="1"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
@@ -2126,13 +2150,11 @@
       <c r="A119" s="1"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="1"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
@@ -2144,11 +2166,13 @@
       <c r="A122" s="1"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
+      <c r="F122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
+      <c r="F123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
@@ -2164,23 +2188,23 @@
       <c r="A126" s="1"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="1"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
+      <c r="F128" s="1"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
+      <c r="F129" s="1"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
@@ -2188,21 +2212,14 @@
       <c r="E130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
+      <c r="A131" s="1"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
-      <c r="G131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
+      <c r="A132" s="1"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
-      <c r="G132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3"/>
@@ -2215,6 +2232,7 @@
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
@@ -2233,6 +2251,8 @@
       <c r="B136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3"/>
@@ -2247,35 +2267,38 @@
       <c r="B138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
-      <c r="F138" s="1"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
-      <c r="F139" s="1"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
+      <c r="F140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
+      <c r="F141" s="1"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
-      <c r="F142" s="1"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
     </row>
@@ -2283,32 +2306,31 @@
       <c r="A144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
+      <c r="F144" s="1"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3"/>
-      <c r="B145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
-      <c r="F145" s="1"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3"/>
-      <c r="B146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
-      <c r="F146" s="1"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
+      <c r="F147" s="1"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
+      <c r="F148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3"/>
@@ -2318,15 +2340,15 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3"/>
+      <c r="B150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
-      <c r="F150" s="1"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3"/>
+      <c r="B151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
-      <c r="F151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3"/>
@@ -2338,20 +2360,21 @@
       <c r="A153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
+      <c r="F153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
+      <c r="F154" s="1"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1"/>
+      <c r="A155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
-      <c r="F155" s="1"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1"/>
+      <c r="A156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
     </row>
@@ -2359,6 +2382,7 @@
       <c r="A157" s="1"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
+      <c r="F157" s="1"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
@@ -2369,7 +2393,6 @@
       <c r="A159" s="1"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
-      <c r="F159" s="1"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
@@ -2380,20 +2403,25 @@
       <c r="A161" s="1"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
+      <c r="F161" s="1"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
     </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J88">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="FR00"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J91"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added H2 demand NOS0, updated VRE, updated demand NO.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -321,13 +321,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E98" activeCellId="0" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,7 +371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -395,7 +395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -418,7 +418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -466,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -507,7 +507,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -524,7 +524,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -542,7 +542,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -560,7 +560,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -577,7 +577,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -594,7 +594,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -611,7 +611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -629,7 +629,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -646,7 +646,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -663,7 +663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -681,7 +681,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -698,7 +698,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -715,7 +715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -788,7 +788,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -806,7 +806,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -823,7 +823,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -857,7 +857,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -874,7 +874,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -891,7 +891,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -908,7 +908,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -925,7 +925,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
@@ -942,7 +942,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
@@ -960,7 +960,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -977,7 +977,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>28</v>
       </c>
@@ -994,7 +994,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>27</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>35</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>30</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>30</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
         <v>17</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>2040</v>
       </c>
       <c r="H64" s="1" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,10 +1550,10 @@
       </c>
       <c r="F66" s="1"/>
       <c r="H66" s="1" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>38</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>38</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>38</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>14</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>26</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>17</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>31</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>31</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
         <v>42</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>43</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>42</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>42</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>42</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
         <v>31</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
         <v>31</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>48000</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>31</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>45</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>45</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>31</v>
       </c>
@@ -2421,7 +2421,20 @@
       <c r="E164" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J91"/>
+  <autoFilter ref="A1:J91">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="2040"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="NOM1"/>
+        <filter val="NON1"/>
+        <filter val="NOS0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added EV units. EV timeseries are not included in this commit. Added possibility to set timeseriesavailability in tech data. Modified loads 2040.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$91</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$98</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="54">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t xml:space="preserve">UK00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EV smart discharger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EV smart charger</t>
   </si>
   <si>
     <t xml:space="preserve">Gas CCGT old 2</t>
@@ -324,10 +330,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J164"/>
+  <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E98" activeCellId="0" sqref="E98"/>
+      <selection pane="topLeft" activeCell="D106" activeCellId="0" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -733,7 +739,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -751,7 +757,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -769,7 +775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -788,7 +794,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -806,7 +812,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -820,10 +826,10 @@
         <v>2040</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -857,7 +863,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -874,7 +880,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -891,7 +897,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1455,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>35</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>35</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>35</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>30</v>
       </c>
@@ -1535,7 +1541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>30</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>45</v>
       </c>
@@ -1988,55 +1994,143 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F92" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H93" s="1" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
+      <c r="A94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="H94" s="1" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
+      <c r="A95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F95" s="1"/>
+      <c r="H95" s="1" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H98" s="1" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
@@ -2084,7 +2178,6 @@
       <c r="A107" s="1"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
-      <c r="F107" s="1"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
@@ -2096,18 +2189,17 @@
       <c r="A109" s="1"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
+      <c r="F109" s="1"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
-      <c r="F110" s="1"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1"/>
@@ -2118,23 +2210,23 @@
       <c r="A113" s="1"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
+      <c r="F113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
+      <c r="F114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
-      <c r="F115" s="1"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="1"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
@@ -2150,11 +2242,13 @@
       <c r="A119" s="1"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
+      <c r="F119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
+      <c r="F120" s="1"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
@@ -2166,13 +2260,11 @@
       <c r="A122" s="1"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
@@ -2188,23 +2280,23 @@
       <c r="A126" s="1"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
+      <c r="F126" s="1"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
+      <c r="F127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="1"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="1"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
@@ -2212,14 +2304,21 @@
       <c r="E130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1"/>
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1"/>
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3"/>
@@ -2232,7 +2331,6 @@
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
@@ -2251,8 +2349,6 @@
       <c r="B136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
-      <c r="F136" s="3"/>
-      <c r="G136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3"/>
@@ -2267,38 +2363,35 @@
       <c r="B138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
+      <c r="F138" s="1"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
-      <c r="F139" s="3"/>
-      <c r="G139" s="3"/>
+      <c r="F139" s="1"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
-      <c r="F140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
-      <c r="F141" s="1"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3"/>
-      <c r="B142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
+      <c r="F142" s="1"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3"/>
-      <c r="B143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
     </row>
@@ -2306,31 +2399,32 @@
       <c r="A144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
-      <c r="F144" s="1"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3"/>
+      <c r="B145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
+      <c r="F145" s="1"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
+      <c r="F146" s="1"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
-      <c r="F147" s="1"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
-      <c r="F148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3"/>
@@ -2340,15 +2434,15 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3"/>
-      <c r="B150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
+      <c r="F150" s="1"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3"/>
-      <c r="B151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
+      <c r="F151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3"/>
@@ -2360,21 +2454,20 @@
       <c r="A153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
-      <c r="F153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
-      <c r="F154" s="1"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="3"/>
+      <c r="A155" s="1"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
+      <c r="F155" s="1"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="3"/>
+      <c r="A156" s="1"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
     </row>
@@ -2382,7 +2475,6 @@
       <c r="A157" s="1"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
-      <c r="F157" s="1"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
@@ -2393,6 +2485,7 @@
       <c r="A159" s="1"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
+      <c r="F159" s="1"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
@@ -2403,35 +2496,25 @@
       <c r="A161" s="1"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
-      <c r="F161" s="1"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="3"/>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J91">
+  <autoFilter ref="A1:J98">
     <filterColumn colId="4">
       <filters>
         <filter val="2040"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="0">
+    <filterColumn colId="2">
       <filters>
-        <filter val="NOM1"/>
-        <filter val="NON1"/>
-        <filter val="NOS0"/>
+        <filter val="DR cutoff tier 1"/>
+        <filter val="DR cutoff tier 2"/>
+        <filter val="DR upwards 1"/>
+        <filter val="DR upwards 2"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2475,7 +2558,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,7 +2574,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2582,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,15 +2590,15 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add scenario spec to unit filters. Adjust EV discharge technology. Add nuclear FI 2040.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$99</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="55">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gas conventional old 2 Bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard coal new Bio</t>
   </si>
 </sst>
 </file>
@@ -332,8 +335,8 @@
   </sheetPr>
   <dimension ref="A1:J162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D106" activeCellId="0" sqref="D106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G92" activeCellId="0" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -401,7 +404,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -415,7 +418,7 @@
         <v>2040</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>3500</v>
+        <v>4320</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -496,7 +499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -513,7 +516,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -530,7 +533,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -548,7 +551,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -566,7 +569,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -794,7 +797,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -829,7 +832,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -846,7 +849,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -863,7 +866,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -880,7 +883,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>2040</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1044,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -1060,7 +1063,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -1079,7 +1082,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1102,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1336,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>14</v>
       </c>
@@ -1960,7 +1963,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>45</v>
       </c>
@@ -1994,7 +1997,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
@@ -2008,10 +2011,10 @@
         <v>2040</v>
       </c>
       <c r="F92" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>2040</v>
       </c>
       <c r="H93" s="1" t="n">
-        <v>10000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,7 +2067,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>16</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>30</v>
       </c>
@@ -2503,18 +2506,10 @@
       <c r="E162" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J98">
-    <filterColumn colId="4">
+  <autoFilter ref="A1:J99">
+    <filterColumn colId="0">
       <filters>
-        <filter val="2040"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="DR cutoff tier 1"/>
-        <filter val="DR cutoff tier 2"/>
-        <filter val="DR upwards 1"/>
-        <filter val="DR upwards 2"/>
+        <filter val="FI00"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2534,10 +2529,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2552,6 +2547,12 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -2560,6 +2561,12 @@
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>2040</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -2568,6 +2575,12 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>2040</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -2576,6 +2589,12 @@
       <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>2040</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
@@ -2584,6 +2603,12 @@
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>2040</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -2591,6 +2616,12 @@
       </c>
       <c r="B6" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>2040</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,13 +2631,137 @@
       <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>2040</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>2040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added EV to DE00. Added some batteries.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$138</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$149</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="55">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -524,7 +524,7 @@
   <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H143" activeCellId="0" sqref="H143"/>
+      <selection pane="topLeft" activeCell="E155" activeCellId="0" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1042,7 +1042,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>29</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>29</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>14</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>14</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>29</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>29</v>
       </c>
@@ -3130,59 +3130,163 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="3"/>
-      <c r="D143" s="3"/>
-      <c r="E143" s="3"/>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="3"/>
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="3"/>
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E143" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F143" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E144" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="H144" s="1" t="n">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B145" s="3"/>
-      <c r="D145" s="3"/>
-      <c r="E145" s="3"/>
-      <c r="F145" s="1"/>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="3"/>
+      <c r="C145" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E145" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F145" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B146" s="3"/>
-      <c r="D146" s="3"/>
-      <c r="E146" s="3"/>
-      <c r="F146" s="1"/>
+      <c r="C146" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E146" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H146" s="1" t="n">
+        <v>500000</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="3"/>
+      <c r="A147" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B147" s="3"/>
-      <c r="D147" s="3"/>
-      <c r="E147" s="3"/>
+      <c r="C147" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E147" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="3"/>
+      <c r="A148" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B148" s="3"/>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="3"/>
+      <c r="C148" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E148" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B149" s="3"/>
-      <c r="D149" s="3"/>
-      <c r="E149" s="3"/>
+      <c r="C149" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E149" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="3"/>
-      <c r="D150" s="3"/>
-      <c r="E150" s="3"/>
-      <c r="F150" s="1"/>
+      <c r="A150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E150" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="3"/>
-      <c r="D151" s="3"/>
-      <c r="E151" s="3"/>
-      <c r="F151" s="1"/>
+      <c r="A151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E151" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3"/>
@@ -3243,11 +3347,10 @@
       <c r="E162" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J138">
+  <autoFilter ref="A1:J149">
     <filterColumn colId="2">
       <filters>
-        <filter val="EV smart charger"/>
-        <filter val="EV smart discharger"/>
+        <filter val="Battery"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added some demand response.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$151</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$158</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="55">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -524,7 +524,7 @@
   <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F158" activeCellId="0" sqref="F158"/>
+      <selection pane="topLeft" activeCell="F70" activeCellId="0" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -904,7 +904,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -921,7 +921,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>2040</v>
       </c>
       <c r="F64" s="1" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +1803,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>29</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>29</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>2030</v>
       </c>
       <c r="F125" s="1" t="n">
-        <v>4500</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,7 +2850,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>14</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>14</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>2030</v>
       </c>
       <c r="F133" s="3" t="n">
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="G133" s="3"/>
     </row>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="G134" s="3"/>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>2030</v>
       </c>
       <c r="F135" s="3" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G135" s="3"/>
     </row>
@@ -3062,7 +3062,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>14</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>14</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>29</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>29</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
         <v>30</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
         <v>30</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
         <v>30</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
         <v>30</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
         <v>35</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
         <v>35</v>
       </c>
@@ -3251,10 +3251,10 @@
         <v>2030</v>
       </c>
       <c r="F149" s="1" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
         <v>30</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
         <v>30</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
         <v>35</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
         <v>35</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
         <v>35</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
         <v>35</v>
       </c>
@@ -3356,20 +3356,54 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="3"/>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1"/>
-      <c r="D157" s="3"/>
-      <c r="E157" s="3"/>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
+      <c r="C156" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E156" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E157" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E158" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1"/>
@@ -3393,12 +3427,18 @@
       <c r="E162" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J151">
+  <autoFilter ref="A1:J158">
     <filterColumn colId="2">
       <filters>
-        <filter val="Battery"/>
-        <filter val="EV smart charger"/>
-        <filter val="EV smart discharger"/>
+        <filter val="DR cutoff tier 1"/>
+        <filter val="DR cutoff tier 2"/>
+        <filter val="Gas CCGT present 1"/>
+        <filter val="Gas OCGT new"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="FI00"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added EV NOS0. Corrected one error in additional units conventional xlsx.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$158</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$164</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="56">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -524,10 +524,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J162"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H161" activeCellId="0" sqref="H161"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E156" activeCellId="0" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -595,7 +595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -672,7 +672,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -777,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -796,7 +796,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -814,7 +814,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -832,7 +832,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -850,7 +850,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -907,7 +907,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -924,7 +924,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -941,7 +941,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -958,7 +958,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -975,7 +975,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -992,7 +992,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>30</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>20</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>21</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>21</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>42</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>24</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>35</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
         <v>30</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>30</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>30</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>42</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>23</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>23</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>24</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>43</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>43</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>35</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>35</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
         <v>44</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>45</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>44</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>44</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>48000</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>37</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>2040</v>
       </c>
       <c r="H93" s="1" t="n">
-        <v>57200</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,7 +2258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>29</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>2040</v>
       </c>
       <c r="F97" s="1" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,10 +2306,10 @@
         <v>2040</v>
       </c>
       <c r="H98" s="1" t="n">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>24</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
         <v>14</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
         <v>19</v>
       </c>
@@ -2406,7 +2406,7 @@
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
         <v>21</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
         <v>21</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
         <v>23</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="s">
         <v>23</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
         <v>24</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
         <v>24</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
         <v>30</v>
       </c>
@@ -2626,7 +2626,7 @@
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
         <v>30</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
         <v>35</v>
       </c>
@@ -2684,7 +2684,7 @@
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
         <v>35</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
         <v>30</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>35</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
         <v>42</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>14</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
         <v>44</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
         <v>42</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>14</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>29</v>
       </c>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="G131" s="3"/>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>24</v>
       </c>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="G132" s="3"/>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>35</v>
       </c>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G133" s="3"/>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
         <v>30</v>
       </c>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="G134" s="3"/>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="G135" s="3"/>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>37</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="G137" s="3"/>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
         <v>24</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>2030</v>
       </c>
       <c r="F141" s="1" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,7 +3239,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
         <v>35</v>
       </c>
@@ -3359,8 +3359,10 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1"/>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="C156" s="1" t="s">
         <v>28</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
         <v>30</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
         <v>30</v>
       </c>
@@ -3408,7 +3410,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>48</v>
       </c>
@@ -3425,7 +3427,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
         <v>48</v>
       </c>
@@ -3443,24 +3445,79 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
+    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E161" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F161" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E162" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H162" s="1" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E163" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F163" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="H164" s="1" t="n">
+        <v>30000</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J158">
+  <autoFilter ref="A1:J164">
     <filterColumn colId="2">
       <filters>
-        <filter val="DR cutoff tier 1"/>
-        <filter val="Electrolysis"/>
-        <filter val="Gas OCGT new"/>
-        <filter val="Hydrogen processor"/>
+        <filter val="DR cutoff tier 2"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Small adjustments to consumption. Added elysis SE03. Adjusted offshore wind SE.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$164</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$165</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="56">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -524,10 +524,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J164"/>
+  <dimension ref="A1:J168"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E156" activeCellId="0" sqref="E156"/>
+      <selection pane="topLeft" activeCell="H167" activeCellId="0" sqref="H167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -672,7 +672,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -689,7 +689,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -924,7 +924,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -941,7 +941,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>29</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>24</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
         <v>19</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
         <v>19</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>29</v>
       </c>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="G134" s="3"/>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="G137" s="3"/>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
         <v>24</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
         <v>35</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
         <v>35</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
         <v>30</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
         <v>30</v>
       </c>
@@ -3513,11 +3513,89 @@
         <v>30000</v>
       </c>
     </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F165" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E166" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H166" s="1" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E167" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F167" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E168" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F168" s="1"/>
+      <c r="H168" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J164">
+  <autoFilter ref="A1:J165">
     <filterColumn colId="2">
       <filters>
-        <filter val="DR cutoff tier 2"/>
+        <filter val="DR cutoff tier 1"/>
+        <filter val="Electrolysis"/>
+        <filter val="Hydrogen processor"/>
+        <filter val="Hydrogen storage dimensioner"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SE01"/>
+        <filter val="SE03"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added more elysis to ES00.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$165</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$168</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J168"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H167" activeCellId="0" sqref="H167"/>
+      <selection pane="topLeft" activeCell="G172" activeCellId="0" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -672,7 +672,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -689,7 +689,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -941,7 +941,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
         <v>19</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
         <v>19</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>29</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>48</v>
       </c>
@@ -3424,10 +3424,10 @@
         <v>2040</v>
       </c>
       <c r="H159" s="1" t="n">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
         <v>48</v>
       </c>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="F160" s="1"/>
       <c r="H160" s="1" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,7 +3513,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
         <v>48</v>
       </c>
@@ -3527,10 +3527,10 @@
         <v>2040</v>
       </c>
       <c r="F165" s="1" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
         <v>29</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
         <v>29</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
         <v>29</v>
       </c>
@@ -3583,7 +3583,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J165">
+  <autoFilter ref="A1:J168">
     <filterColumn colId="2">
       <filters>
         <filter val="DR cutoff tier 1"/>
@@ -3594,8 +3594,7 @@
     </filterColumn>
     <filterColumn colId="0">
       <filters>
-        <filter val="SE01"/>
-        <filter val="SE03"/>
+        <filter val="ES00"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added EV UK00. Updates authors.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="56">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -524,10 +524,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J168"/>
+  <dimension ref="A1:J172"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F172" activeCellId="0" sqref="F172"/>
+      <selection pane="topLeft" activeCell="F174" activeCellId="0" sqref="F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -614,7 +614,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
         <v>14</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>14</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>14</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>48</v>
       </c>
@@ -3582,19 +3582,88 @@
         <v>500</v>
       </c>
     </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E169" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F169" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E170" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="H170" s="1" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E171" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F171" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E172" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H172" s="1" t="n">
+        <v>400000</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J168">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Electrolysis"/>
-        <filter val="Electrolysis Raahe"/>
-        <filter val="Hydrogen processor"/>
-        <filter val="Hydrogen storage dimensioner"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="0">
       <filters>
         <filter val="ES00"/>
+        <filter val="FI00"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="EV smart charger"/>
+        <filter val="EV smart discharger"/>
+        <filter val="Hydrogen processor"/>
+        <filter val="Hydrogen storage dimensioner"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added some condensing capacity in FR00.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="57">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -3709,26 +3709,16 @@
       <c r="E175" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="F175" s="0" t="n">
+      <c r="F175" s="1" t="n">
         <v>2600</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D176" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E176" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F176" s="0" t="n">
-        <v>1000</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="3"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J174">

</xml_diff>

<commit_message>
Added some batteries in FR00 UK00.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$174</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$175</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="57">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -527,10 +527,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J176"/>
+  <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F180" activeCellId="0" sqref="F180"/>
+      <selection pane="topLeft" activeCell="F178" activeCellId="0" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1048,7 +1048,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
         <v>35</v>
       </c>
@@ -3714,22 +3714,50 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="3"/>
-      <c r="E176" s="3"/>
-      <c r="F176" s="1"/>
+      <c r="A176" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E176" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F176" s="1" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B177" s="3"/>
+      <c r="C177" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E177" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>1200</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J174">
+  <autoFilter ref="A1:J175">
     <filterColumn colId="4">
       <filters>
         <filter val="2025"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="0">
+    <filterColumn colId="2">
       <filters>
-        <filter val="FR00"/>
+        <filter val="Battery"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update of solar PV in DE00 2030->.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -529,8 +529,8 @@
   </sheetPr>
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I52" activeCellId="0" sqref="I52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G79" activeCellId="0" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1737,7 +1737,7 @@
         <v>2040</v>
       </c>
       <c r="H65" s="1" t="n">
-        <v>9000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F67" s="1"/>
       <c r="H67" s="1" t="n">
-        <v>3000</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="F82" s="1"/>
       <c r="H82" s="1" t="n">
-        <v>4000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2118,7 +2118,7 @@
         <v>2040</v>
       </c>
       <c r="H87" s="1" t="n">
-        <v>2000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="F89" s="1"/>
       <c r="H89" s="1" t="n">
-        <v>1000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Increased batteries in FR00, DE00.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$177</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$173</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="57">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -527,10 +527,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J177"/>
+  <dimension ref="A1:J173"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H81" activeCellId="0" sqref="H81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B181" activeCellId="0" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1305,7 +1305,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>20</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>34</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>21</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
         <v>21</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>21</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>30</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
         <v>30</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>30</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>23</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>23</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>23</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>24</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>24</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>43</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>43</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>43</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>35</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>35</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>35</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>45</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>45</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>44</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>44</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>44</v>
       </c>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="B147" s="3"/>
       <c r="C147" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>39</v>
@@ -3224,34 +3224,32 @@
         <v>2030</v>
       </c>
       <c r="F147" s="1" t="n">
-        <v>600</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B148" s="3"/>
       <c r="C148" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E148" s="3" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="F148" s="1" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B149" s="3"/>
       <c r="C149" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>39</v>
@@ -3259,33 +3257,33 @@
       <c r="E149" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="F149" s="1" t="n">
-        <v>4000</v>
+      <c r="H149" s="1" t="n">
+        <v>150000</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
-        <v>30</v>
+      <c r="A150" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E150" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F150" s="1" t="n">
-        <v>600</v>
+        <v>900</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
-        <v>30</v>
+      <c r="A151" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>39</v>
@@ -3293,8 +3291,8 @@
       <c r="E151" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F151" s="1" t="n">
-        <v>1000</v>
+      <c r="H151" s="1" t="n">
+        <v>300000</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,24 +3300,24 @@
         <v>35</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E152" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F152" s="1" t="n">
-        <v>300</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>39</v>
@@ -3327,136 +3325,136 @@
       <c r="E153" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="H153" s="1" t="n">
-        <v>150000</v>
+      <c r="F153" s="1" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E154" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F154" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E155" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H155" s="1" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E156" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F156" s="1"/>
+      <c r="H156" s="1" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C157" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D154" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E154" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F154" s="1" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C155" s="1" t="s">
+      <c r="D157" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E157" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F157" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D155" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E155" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="H155" s="1" t="n">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E156" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F156" s="1" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E157" s="3" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F157" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D158" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E158" s="3" t="n">
         <v>2040</v>
       </c>
-      <c r="F158" s="1" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H158" s="1" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="H159" s="1" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2030</v>
+      </c>
+      <c r="F159" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E160" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F160" s="1"/>
+        <v>2030</v>
+      </c>
       <c r="H160" s="1" t="n">
-        <v>4000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>39</v>
@@ -3465,15 +3463,15 @@
         <v>2040</v>
       </c>
       <c r="F161" s="1" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>39</v>
@@ -3482,83 +3480,84 @@
         <v>2040</v>
       </c>
       <c r="H162" s="1" t="n">
-        <v>50000</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F163" s="1" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C164" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F164" s="1"/>
+      <c r="H164" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F165" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C166" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E164" s="3" t="n">
-        <v>2030</v>
-      </c>
-      <c r="H164" s="1" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E165" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F165" s="1" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D166" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E166" s="3" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="H166" s="1" t="n">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>39</v>
@@ -3567,199 +3566,129 @@
         <v>2040</v>
       </c>
       <c r="F167" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C168" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E168" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H168" s="1" t="n">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B169" s="4"/>
+      <c r="C169" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D168" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E168" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F168" s="1"/>
-      <c r="H168" s="1" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D169" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E169" s="3" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F169" s="1" t="n">
+      <c r="D169" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E169" s="4" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
+      <c r="H169" s="4" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E170" s="3" t="n">
-        <v>2030</v>
-      </c>
-      <c r="H170" s="1" t="n">
-        <v>200000</v>
+      <c r="A170" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B170" s="4"/>
+      <c r="C170" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E170" s="4" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
+      <c r="H170" s="4" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="F171" s="1" t="n">
-        <v>600</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E172" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F172" s="1" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E172" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="H172" s="1" t="n">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B173" s="4"/>
-      <c r="C173" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D173" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E173" s="4" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F173" s="4"/>
-      <c r="G173" s="4"/>
-      <c r="H173" s="4" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B174" s="4"/>
-      <c r="C174" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D174" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E174" s="4" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F174" s="4"/>
-      <c r="G174" s="4"/>
-      <c r="H174" s="4" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E175" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F175" s="1" t="n">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C176" s="1" t="s">
+      <c r="B173" s="3"/>
+      <c r="C173" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D176" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E176" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F176" s="1" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B177" s="3"/>
-      <c r="C177" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E177" s="3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F177" s="1" t="n">
+      <c r="D173" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E173" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F173" s="1" t="n">
         <v>1200</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J177">
+  <autoFilter ref="A1:J173">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Battery"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
+        <filter val="2030"/>
         <filter val="2040"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Electrolysis"/>
-        <filter val="Hydrogen processor"/>
-        <filter val="Hydrogen storage dimensioner"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Increased batteries and PV in PL00.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-conventional.xlsx
+++ b/input/capacity/additional-units-conventional.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$173</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$174</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="57">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -527,10 +527,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J173"/>
+  <dimension ref="A1:J176"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B181" activeCellId="0" sqref="B181"/>
+      <selection pane="topLeft" activeCell="F177" activeCellId="0" sqref="F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1048,7 +1048,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
         <v>35</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="3" t="s">
         <v>37</v>
       </c>
@@ -3678,17 +3678,62 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E174" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F174" s="1" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E175" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E176" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>5000</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J173">
+  <autoFilter ref="A1:J174">
     <filterColumn colId="2">
       <filters>
         <filter val="Battery"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="2030"/>
-        <filter val="2040"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>